<commit_message>
correcting the nonlinear 2d results
</commit_message>
<xml_diff>
--- a/graphs/path_errors.xlsx
+++ b/graphs/path_errors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="1800" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t xml:space="preserve">Benchmark </t>
   </si>
   <si>
-    <t>simpleInterpolator</t>
-  </si>
-  <si>
     <t>squareRoot (Fluctuat)</t>
   </si>
   <si>
@@ -111,23 +108,48 @@
     <t>&amp;</t>
   </si>
   <si>
-    <t xml:space="preserve">linear fit </t>
-  </si>
-  <si>
-    <t>quadratic fit</t>
-  </si>
-  <si>
     <t>~150</t>
   </si>
   <si>
     <t>~50</t>
+  </si>
+  <si>
+    <t>simpleInterpolator (float)</t>
+  </si>
+  <si>
+    <t>quadratic fit (Piecewise2D)</t>
+  </si>
+  <si>
+    <t>linear fit (Piecewise2D)</t>
+  </si>
+  <si>
+    <t>quadratic fit (Piecewise2D,
+ x+/-1e-8 &amp;&amp; y+/-1e-8)</t>
+  </si>
+  <si>
+    <t>~735</t>
+  </si>
+  <si>
+    <t>~100</t>
+  </si>
+  <si>
+    <t>!0.6305252000000009</t>
+  </si>
+  <si>
+    <t>!0.6305252076631006</t>
+  </si>
+  <si>
+    <t>!3.217784400701105</t>
+  </si>
+  <si>
+    <t>!3.2177844000000015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -165,6 +187,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -192,7 +220,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -202,8 +230,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -228,16 +260,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -570,12 +610,12 @@
   <dimension ref="A2:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" customWidth="1"/>
@@ -586,7 +626,7 @@
   <sheetData>
     <row r="2" spans="1:11" ht="20">
       <c r="A2" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -599,31 +639,31 @@
     </row>
     <row r="4" spans="1:11" s="7" customFormat="1" ht="20">
       <c r="A4" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="D4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="7" customFormat="1" ht="20">
@@ -634,36 +674,36 @@
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="20">
       <c r="A6" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="20"/>
     <row r="9" spans="1:11">
       <c r="C9" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="I9" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
@@ -674,30 +714,30 @@
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="K10" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -705,25 +745,25 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="5">
-        <v>2.251E-5</v>
+        <v>2.51822175501656E-5</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="5">
-        <v>3.400001E-5</v>
+        <v>3.6682214426411101E-5</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I12" s="2">
         <v>1.5</v>
@@ -740,25 +780,25 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>2.328647E-2</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14">
         <v>2.380814039E-2</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I14" s="2">
         <v>3</v>
@@ -775,22 +815,22 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5">
         <v>7.0337550000000001E-12</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="5">
         <v>8.5789979999999993E-12</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I16" s="2">
         <v>82.5</v>
@@ -807,22 +847,22 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="5">
         <v>3.750028E-11</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="5">
         <v>7.5000219999999997E-11</v>
       </c>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I18" s="2">
         <v>6</v>
@@ -839,22 +879,22 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="5">
         <v>1.2499378000000001E-9</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20" s="5">
         <v>1.312439E-9</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I20" s="2">
         <v>7.2</v>
@@ -871,22 +911,22 @@
     </row>
     <row r="22" spans="1:11" ht="16" thickBot="1">
       <c r="A22" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="4">
         <v>2.9000000000000101</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -903,10 +943,10 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E24" s="5">
         <v>2.3350917490834502E-9</v>
@@ -924,7 +964,7 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C26">
         <v>1.9814240000000001</v>
@@ -947,7 +987,7 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C28">
         <v>3.2177844000000002</v>
@@ -956,24 +996,49 @@
         <v>0.63052520000000001</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11">
+      <c r="C29" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11">
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
+    <row r="30" spans="1:11" ht="30">
+      <c r="A30" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30">
+        <v>3.2177845</v>
+      </c>
+      <c r="E30">
+        <v>0.63052529999999996</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11">
+      <c r="C31" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>

</xml_diff>